<commit_message>
Final files Hw 8
</commit_message>
<xml_diff>
--- a/Hw_8/FOPTD_Fits.xlsx
+++ b/Hw_8/FOPTD_Fits.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\austin.utexas.edu\disk\engrstu\che\kr27867\Desktop\Hw 8 process\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\austin.utexas.edu\disk\engrstu\CHE\kr27867\Desktop\Hw 8 process\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ca0" sheetId="2" r:id="rId1"/>
@@ -17,24 +17,60 @@
     <sheet name="Tc" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Ca0!$L$5:$L$7</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">Tc!$L$5:$L$7</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Tf!$L$5:$L$7</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">Tf!$L$5</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Tf!$L$7</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">Tf!$L$7</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Ca0!$L$4</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Tc!$L$4</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Tf!$L$4</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
@@ -42,16 +78,36 @@
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">Tf!$L$6</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -860,130 +916,130 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5106815446127851E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.1345132080654209E-5</c:v>
+                  <c:v>5.5469438651942637E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.3395310547987209E-4</c:v>
+                  <c:v>1.2452526767073275E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.7573555113656352E-4</c:v>
+                  <c:v>1.7664258920160292E-4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.0892011713013453E-4</c:v>
+                  <c:v>2.1597620147078615E-4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3527605208975569E-4</c:v>
+                  <c:v>2.4566178408895744E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6784498142919577E-4</c:v>
+                  <c:v>2.7999230424755739E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.8998632532677555E-4</c:v>
+                  <c:v>3.0141930310782279E-4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.0503868103922495E-4</c:v>
+                  <c:v>3.1479271772655797E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.1527172802779912E-4</c:v>
+                  <c:v>3.2313958047345729E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.2222846308447575E-4</c:v>
+                  <c:v>3.2834917874748158E-4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.269578621288496E-4</c:v>
+                  <c:v>3.3160068952460558E-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.3033506863360955E-4</c:v>
+                  <c:v>3.3372751217563255E-4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.3257650863903097E-4</c:v>
+                  <c:v>3.3501656589124927E-4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.3406414443826963E-4</c:v>
+                  <c:v>3.3579785317015912E-4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.3505148305354552E-4</c:v>
+                  <c:v>3.3627138643319661E-4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.3570677619835544E-4</c:v>
+                  <c:v>3.365583919396932E-4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.3614169193951169E-4</c:v>
+                  <c:v>3.3673234415633588E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.3643034397776904E-4</c:v>
+                  <c:v>3.3683777549124033E-4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.3670398018959891E-4</c:v>
+                  <c:v>3.3692707771559085E-4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.3684617431444555E-4</c:v>
+                  <c:v>3.3696722036883264E-4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.3692006500678375E-4</c:v>
+                  <c:v>3.3698526507736044E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.3695846205321659E-4</c:v>
+                  <c:v>3.369933764372123E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.3697841494752722E-4</c:v>
+                  <c:v>3.3699702261185381E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3698878340105061E-4</c:v>
+                  <c:v>3.3699866162057232E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.369948171020925E-4</c:v>
+                  <c:v>3.3699947876709941E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.3699760511801837E-4</c:v>
+                  <c:v>3.3699979700544481E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.3699889338748159E-4</c:v>
+                  <c:v>3.3699992094361384E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.369994886632096E-4</c:v>
+                  <c:v>3.3699996921142942E-4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.36999763724602E-4</c:v>
+                  <c:v>3.3699998800936745E-4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.3699989082329934E-4</c:v>
+                  <c:v>3.369999953302389E-4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.3699996694174118E-4</c:v>
+                  <c:v>3.3699999891474692E-4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.3699998999009434E-4</c:v>
+                  <c:v>3.3699999974778704E-4</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.3699999696904144E-4</c:v>
+                  <c:v>3.3699999994138565E-4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.3699999908223815E-4</c:v>
+                  <c:v>3.3699999998637804E-4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.3699999972210549E-4</c:v>
+                  <c:v>3.3699999999683424E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.369999999694506E-4</c:v>
+                  <c:v>3.3699999999978658E-4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.3699999999664164E-4</c:v>
+                  <c:v>3.3699999999998559E-4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.3699999999963078E-4</c:v>
+                  <c:v>3.3699999999999903E-4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.369999999999594E-4</c:v>
+                  <c:v>3.3699999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.3699999999999556E-4</c:v>
+                  <c:v>3.3700000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.3699999999999995E-4</c:v>
+                  <c:v>3.3700000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>3.3700000000000001E-4</c:v>
@@ -1814,130 +1870,130 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5106815446127851E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.1345132080654209E-5</c:v>
+                  <c:v>5.5469438651942637E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.3395310547987209E-4</c:v>
+                  <c:v>1.2452526767073275E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.7573555113656352E-4</c:v>
+                  <c:v>1.7664258920160292E-4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.0892011713013453E-4</c:v>
+                  <c:v>2.1597620147078615E-4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3527605208975569E-4</c:v>
+                  <c:v>2.4566178408895744E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6784498142919577E-4</c:v>
+                  <c:v>2.7999230424755739E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.8998632532677555E-4</c:v>
+                  <c:v>3.0141930310782279E-4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.0503868103922495E-4</c:v>
+                  <c:v>3.1479271772655797E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.1527172802779912E-4</c:v>
+                  <c:v>3.2313958047345729E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.2222846308447575E-4</c:v>
+                  <c:v>3.2834917874748158E-4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.269578621288496E-4</c:v>
+                  <c:v>3.3160068952460558E-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.3033506863360955E-4</c:v>
+                  <c:v>3.3372751217563255E-4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.3257650863903097E-4</c:v>
+                  <c:v>3.3501656589124927E-4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.3406414443826963E-4</c:v>
+                  <c:v>3.3579785317015912E-4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.3505148305354552E-4</c:v>
+                  <c:v>3.3627138643319661E-4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.3570677619835544E-4</c:v>
+                  <c:v>3.365583919396932E-4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.3614169193951169E-4</c:v>
+                  <c:v>3.3673234415633588E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.3643034397776904E-4</c:v>
+                  <c:v>3.3683777549124033E-4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.3670398018959891E-4</c:v>
+                  <c:v>3.3692707771559085E-4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.3684617431444555E-4</c:v>
+                  <c:v>3.3696722036883264E-4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.3692006500678375E-4</c:v>
+                  <c:v>3.3698526507736044E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.3695846205321659E-4</c:v>
+                  <c:v>3.369933764372123E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.3697841494752722E-4</c:v>
+                  <c:v>3.3699702261185381E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3698878340105061E-4</c:v>
+                  <c:v>3.3699866162057232E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.369948171020925E-4</c:v>
+                  <c:v>3.3699947876709941E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.3699760511801837E-4</c:v>
+                  <c:v>3.3699979700544481E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.3699889338748159E-4</c:v>
+                  <c:v>3.3699992094361384E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.369994886632096E-4</c:v>
+                  <c:v>3.3699996921142942E-4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.36999763724602E-4</c:v>
+                  <c:v>3.3699998800936745E-4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.3699989082329934E-4</c:v>
+                  <c:v>3.369999953302389E-4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.3699996694174118E-4</c:v>
+                  <c:v>3.3699999891474692E-4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.3699998999009434E-4</c:v>
+                  <c:v>3.3699999974778704E-4</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.3699999696904144E-4</c:v>
+                  <c:v>3.3699999994138565E-4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.3699999908223815E-4</c:v>
+                  <c:v>3.3699999998637804E-4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.3699999972210549E-4</c:v>
+                  <c:v>3.3699999999683424E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.369999999694506E-4</c:v>
+                  <c:v>3.3699999999978658E-4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.3699999999664164E-4</c:v>
+                  <c:v>3.3699999999998559E-4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.3699999999963078E-4</c:v>
+                  <c:v>3.3699999999999903E-4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.369999999999594E-4</c:v>
+                  <c:v>3.3699999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.3699999999999556E-4</c:v>
+                  <c:v>3.3700000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.3699999999999995E-4</c:v>
+                  <c:v>3.3700000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>3.3700000000000001E-4</c:v>
@@ -2768,130 +2824,130 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5106815446127851E-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.1345132080654209E-5</c:v>
+                  <c:v>5.5469438651942637E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.3395310547987209E-4</c:v>
+                  <c:v>1.2452526767073275E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.7573555113656352E-4</c:v>
+                  <c:v>1.7664258920160292E-4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.0892011713013453E-4</c:v>
+                  <c:v>2.1597620147078615E-4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3527605208975569E-4</c:v>
+                  <c:v>2.4566178408895744E-4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6784498142919577E-4</c:v>
+                  <c:v>2.7999230424755739E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.8998632532677555E-4</c:v>
+                  <c:v>3.0141930310782279E-4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.0503868103922495E-4</c:v>
+                  <c:v>3.1479271772655797E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.1527172802779912E-4</c:v>
+                  <c:v>3.2313958047345729E-4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.2222846308447575E-4</c:v>
+                  <c:v>3.2834917874748158E-4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.269578621288496E-4</c:v>
+                  <c:v>3.3160068952460558E-4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.3033506863360955E-4</c:v>
+                  <c:v>3.3372751217563255E-4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.3257650863903097E-4</c:v>
+                  <c:v>3.3501656589124927E-4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.3406414443826963E-4</c:v>
+                  <c:v>3.3579785317015912E-4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.3505148305354552E-4</c:v>
+                  <c:v>3.3627138643319661E-4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.3570677619835544E-4</c:v>
+                  <c:v>3.365583919396932E-4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.3614169193951169E-4</c:v>
+                  <c:v>3.3673234415633588E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.3643034397776904E-4</c:v>
+                  <c:v>3.3683777549124033E-4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.3670398018959891E-4</c:v>
+                  <c:v>3.3692707771559085E-4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.3684617431444555E-4</c:v>
+                  <c:v>3.3696722036883264E-4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.3692006500678375E-4</c:v>
+                  <c:v>3.3698526507736044E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.3695846205321659E-4</c:v>
+                  <c:v>3.369933764372123E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.3697841494752722E-4</c:v>
+                  <c:v>3.3699702261185381E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3698878340105061E-4</c:v>
+                  <c:v>3.3699866162057232E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.369948171020925E-4</c:v>
+                  <c:v>3.3699947876709941E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.3699760511801837E-4</c:v>
+                  <c:v>3.3699979700544481E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.3699889338748159E-4</c:v>
+                  <c:v>3.3699992094361384E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.369994886632096E-4</c:v>
+                  <c:v>3.3699996921142942E-4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.36999763724602E-4</c:v>
+                  <c:v>3.3699998800936745E-4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.3699989082329934E-4</c:v>
+                  <c:v>3.369999953302389E-4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.3699996694174118E-4</c:v>
+                  <c:v>3.3699999891474692E-4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.3699998999009434E-4</c:v>
+                  <c:v>3.3699999974778704E-4</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.3699999696904144E-4</c:v>
+                  <c:v>3.3699999994138565E-4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.3699999908223815E-4</c:v>
+                  <c:v>3.3699999998637804E-4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.3699999972210549E-4</c:v>
+                  <c:v>3.3699999999683424E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.369999999694506E-4</c:v>
+                  <c:v>3.3699999999978658E-4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.3699999999664164E-4</c:v>
+                  <c:v>3.3699999999998559E-4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.3699999999963078E-4</c:v>
+                  <c:v>3.3699999999999903E-4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.369999999999594E-4</c:v>
+                  <c:v>3.3699999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.3699999999999556E-4</c:v>
+                  <c:v>3.3700000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.3699999999999995E-4</c:v>
+                  <c:v>3.3700000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>3.3700000000000001E-4</c:v>
@@ -5131,8 +5187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5208,15 +5264,15 @@
         <v>0.91236044015048701</v>
       </c>
       <c r="D3" s="6">
-        <f t="shared" ref="D3:D55" si="0">C3-0.9115</f>
+        <f t="shared" ref="D3:D66" si="0">C3-0.9115</f>
         <v>8.604401504870296E-4</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G55" si="1">$L$5*(1-EXP(-(IF(A3&lt;$L$6,0,A3-$L$6))/$L$7))</f>
+        <f t="shared" ref="G3:G66" si="1">$L$5*(1-EXP(-(IF(A3&lt;$L$6,0,A3-$L$6))/$L$7))</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H55" si="2">(D3-G3)^2</f>
+        <f t="shared" ref="H3:H66" si="2">(D3-G3)^2</f>
         <v>7.4035725257014209E-7</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -5250,7 +5306,7 @@
       </c>
       <c r="L4">
         <f>SUM(H2:H1048576)</f>
-        <v>9.5158524844934477E-4</v>
+        <v>1.5104542545178183E-5</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -5279,14 +5335,14 @@
         <v>11</v>
       </c>
       <c r="L5">
-        <v>3.3700000000000001E-4</v>
+        <v>6.2278273491840671E-3</v>
       </c>
       <c r="M5" t="s">
         <v>13</v>
       </c>
       <c r="N5">
-        <f>L5/0.1</f>
-        <v>3.3699999999999997E-3</v>
+        <f>L5/0.01</f>
+        <v>0.62278273491840674</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -5315,7 +5371,7 @@
         <v>8</v>
       </c>
       <c r="L6">
-        <v>0.18345490273341014</v>
+        <v>0.26669999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -5344,7 +5400,7 @@
         <v>9</v>
       </c>
       <c r="L7">
-        <v>0.2251183179597776</v>
+        <v>0.23581002712361893</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -5616,11 +5672,11 @@
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>8.3720124189070084E-6</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
-        <v>4.0138004860213341E-7</v>
+        <v>4.1205824273813418E-7</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -5639,11 +5695,11 @@
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>5.965504975787341E-5</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
-        <v>7.0554213336325094E-7</v>
+        <v>8.0931723226586243E-7</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -5662,11 +5718,11 @@
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>1.029352692660512E-4</v>
+        <v>0</v>
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
-        <v>1.2495294852369011E-6</v>
+        <v>1.4902520907776377E-6</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -5685,11 +5741,11 @@
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>1.3946152624835377E-4</v>
+        <v>9.044170573042716E-4</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
-        <v>2.1042940736837897E-6</v>
+        <v>4.7013372642756016E-7</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5708,11 +5764,11 @@
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>1.6504023812375317E-4</v>
+        <v>1.5645022042767391E-3</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
-        <v>3.0716910814815843E-6</v>
+        <v>1.2472346166716564E-7</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5731,11 +5787,11 @@
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>1.8730683318069722E-4</v>
+        <v>2.1427389913889171E-3</v>
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
-        <v>4.2986138718009262E-6</v>
+        <v>1.3895158050723275E-8</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -5754,11 +5810,11 @@
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>2.0669018828650299E-4</v>
+        <v>2.6492763426736597E-3</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
-        <v>5.7869162138403031E-6</v>
+        <v>1.3679009894796553E-9</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -5777,11 +5833,11 @@
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>2.2356364622638553E-4</v>
+        <v>3.0930047493839203E-3</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>7.5245501985410498E-6</v>
+        <v>1.5964258091850164E-8</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -5800,11 +5856,11 @@
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>2.382522066585124E-4</v>
+        <v>3.4817123114664604E-3</v>
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>9.4868967120130304E-6</v>
+        <v>2.6692851477709054E-8</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -5823,11 +5879,11 @@
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>2.5417256234187114E-4</v>
+        <v>3.9060133108592761E-3</v>
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>1.2241855161269151E-5</v>
+        <v>2.3410374075910298E-8</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -5846,11 +5902,11 @@
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>2.6752620016240014E-4</v>
+        <v>4.2647557536683355E-3</v>
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
-        <v>1.5212511232771478E-5</v>
+        <v>9.3910856268204549E-9</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -5869,11 +5925,11 @@
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>2.7872693251967061E-4</v>
+        <v>4.5680690629859421E-3</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>1.830046104965058E-5</v>
+        <v>1.30835062687171E-10</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -5892,11 +5948,11 @@
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>2.8812185598736765E-4</v>
+        <v>4.8245175692982287E-3</v>
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>2.1405889077123157E-5</v>
+        <v>8.1458139223633283E-9</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -5915,11 +5971,11 @@
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>2.9600210739848053E-4</v>
+        <v>5.0413423322397529E-3</v>
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>2.4434942818243372E-5</v>
+        <v>3.9137146989132262E-8</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -5938,11 +5994,11 @@
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>3.0261188580868952E-4</v>
+        <v>5.2246655985776786E-3</v>
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>2.7305473910288159E-5</v>
+        <v>9.205779630045077E-8</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -5961,11 +6017,11 @@
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>3.1219063924263268E-4</v>
+        <v>5.4933014503615006E-3</v>
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>3.2000812188273591E-5</v>
+        <v>2.2640012919587865E-7</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -5984,11 +6040,11 @@
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>3.1910124644332112E-4</v>
+        <v>5.6899995305745906E-3</v>
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
-        <v>3.5662640324917443E-5</v>
+        <v>3.6110753374505371E-7</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -6007,11 +6063,11 @@
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>3.2408691521656439E-4</v>
+        <v>5.8340239953010992E-3</v>
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
-        <v>3.8213619756701845E-5</v>
+        <v>4.5128768360241033E-7</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -6030,11 +6086,11 @@
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
-        <v>3.2768383403927167E-4</v>
+        <v>5.9394802682717638E-3</v>
       </c>
       <c r="H37">
         <f t="shared" si="2"/>
-        <v>3.9723148671247031E-5</v>
+        <v>4.7725142710647136E-7</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -6053,11 +6109,11 @@
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
-        <v>3.2976559682684189E-4</v>
+        <v>6.0013311148328233E-3</v>
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
-        <v>4.0275669172651193E-5</v>
+        <v>4.5528208892985232E-7</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -6076,11 +6132,11 @@
       </c>
       <c r="G39">
         <f t="shared" si="1"/>
-        <v>3.3138217508227915E-4</v>
+        <v>6.0499148694981783E-3</v>
       </c>
       <c r="H39">
         <f t="shared" si="2"/>
-        <v>4.0390992203028002E-5</v>
+        <v>4.0558824487483305E-7</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -6099,11 +6155,11 @@
       </c>
       <c r="G40">
         <f t="shared" si="1"/>
-        <v>3.3263751756008555E-4</v>
+        <v>6.0880773417782315E-3</v>
       </c>
       <c r="H40">
         <f t="shared" si="2"/>
-        <v>4.0166068615952318E-5</v>
+        <v>3.3899267459994243E-7</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -6122,11 +6178,11 @@
       </c>
       <c r="G41">
         <f t="shared" si="1"/>
-        <v>3.3361234493468639E-4</v>
+        <v>6.1180539111182703E-3</v>
       </c>
       <c r="H41">
         <f t="shared" si="2"/>
-        <v>3.9693024224762171E-5</v>
+        <v>2.6604803801297623E-7</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -6145,11 +6201,11 @@
       </c>
       <c r="G42">
         <f t="shared" si="1"/>
-        <v>3.3436934027824525E-4</v>
+        <v>6.1416004649894069E-3</v>
       </c>
       <c r="H42">
         <f t="shared" si="2"/>
-        <v>3.9053942882158838E-5</v>
+        <v>1.954385003372446E-7</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -6168,11 +6224,11 @@
       </c>
       <c r="G43">
         <f t="shared" si="1"/>
-        <v>3.3495717968971497E-4</v>
+        <v>6.1600962505783874E-3</v>
       </c>
       <c r="H43">
         <f t="shared" si="2"/>
-        <v>3.8318470228203002E-5</v>
+        <v>1.3326324188617807E-7</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -6191,11 +6247,11 @@
       </c>
       <c r="G44">
         <f t="shared" si="1"/>
-        <v>3.3541366225148668E-4</v>
+        <v>6.1746246646480468E-3</v>
       </c>
       <c r="H44">
         <f t="shared" si="2"/>
-        <v>3.7543232161561673E-5</v>
+        <v>8.2968325682685467E-8</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -6214,11 +6270,11 @@
       </c>
       <c r="G45">
         <f t="shared" si="1"/>
-        <v>3.359658307518656E-4</v>
+        <v>6.1924639561692892E-3</v>
       </c>
       <c r="H45">
         <f t="shared" si="2"/>
-        <v>3.6259780762144742E-5</v>
+        <v>2.7261760303754266E-8</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -6237,11 +6293,11 @@
       </c>
       <c r="G46">
         <f t="shared" si="1"/>
-        <v>3.3632580181314523E-4</v>
+        <v>6.2043215885927757E-3</v>
       </c>
       <c r="H46">
         <f t="shared" si="2"/>
-        <v>3.5126073246657087E-5</v>
+        <v>3.449160330883293E-9</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -6260,11 +6316,11 @@
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
-        <v>3.3651673522036753E-4</v>
+        <v>6.2107221475409501E-3</v>
       </c>
       <c r="H47">
         <f t="shared" si="2"/>
-        <v>3.4392044587708775E-5</v>
+        <v>9.4718156873417235E-11</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -6283,11 +6339,11 @@
       </c>
       <c r="G48">
         <f t="shared" si="1"/>
-        <v>3.3665359615052843E-4</v>
+        <v>6.2153798505330303E-3</v>
       </c>
       <c r="H48">
         <f t="shared" si="2"/>
-        <v>3.3800223236256515E-5</v>
+        <v>4.2159456778310645E-9</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -6306,11 +6362,11 @@
       </c>
       <c r="G49">
         <f t="shared" si="1"/>
-        <v>3.3675169796768559E-4</v>
+        <v>6.2187692728222542E-3</v>
       </c>
       <c r="H49">
         <f t="shared" si="2"/>
-        <v>3.3347998684090006E-5</v>
+        <v>1.1501482730242408E-8</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -6329,11 +6385,11 @@
       </c>
       <c r="G50">
         <f t="shared" si="1"/>
-        <v>3.36822017280277E-4</v>
+        <v>6.2212357640249391E-3</v>
       </c>
       <c r="H50">
         <f t="shared" si="2"/>
-        <v>3.3024152623555058E-5</v>
+        <v>1.8974861019361378E-8</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -6352,11 +6408,11 @@
       </c>
       <c r="G51">
         <f t="shared" si="1"/>
-        <v>3.3687242211340466E-4</v>
+        <v>6.2230306359334258E-3</v>
       </c>
       <c r="H51">
         <f t="shared" si="2"/>
-        <v>3.2812205578498889E-5</v>
+        <v>2.4952718304782943E-8</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -6375,11 +6431,11 @@
       </c>
       <c r="G52">
         <f t="shared" si="1"/>
-        <v>3.3690855226185183E-4</v>
+        <v>6.2243367687768612E-3</v>
       </c>
       <c r="H52">
         <f t="shared" si="2"/>
-        <v>3.2693119065241614E-5</v>
+        <v>2.8777225934863672E-8</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -6398,11 +6454,11 @@
       </c>
       <c r="G53">
         <f t="shared" si="1"/>
-        <v>3.3693728362576262E-4</v>
+        <v>6.2253921639083224E-3</v>
       </c>
       <c r="H53">
         <f t="shared" si="2"/>
-        <v>3.2645616643450579E-5</v>
+        <v>3.0562243572532585E-8</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -6421,11 +6477,11 @@
       </c>
       <c r="G54">
         <f t="shared" si="1"/>
-        <v>3.3695698807125103E-4</v>
+        <v>6.226128454835448E-3</v>
       </c>
       <c r="H54">
         <f t="shared" si="2"/>
-        <v>3.2665230853712082E-5</v>
+        <v>3.0213743210937028E-8</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -6444,11 +6500,11 @@
       </c>
       <c r="G55">
         <f t="shared" si="1"/>
-        <v>3.3697050170649684E-4</v>
+        <v>6.226642124373241E-3</v>
       </c>
       <c r="H55">
         <f t="shared" si="2"/>
-        <v>3.272845242562759E-5</v>
+        <v>2.8491070642908452E-8</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -6461,6 +6517,18 @@
       <c r="C56" s="6">
         <v>0.91756548179138497</v>
       </c>
+      <c r="D56" s="6">
+        <f t="shared" si="0"/>
+        <v>6.0654817913849968E-3</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="1"/>
+        <v>6.2270004832560366E-3</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="2"/>
+        <v>2.6088287823731925E-8</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
@@ -6472,6 +6540,18 @@
       <c r="C57" s="6">
         <v>0.91757385778538203</v>
       </c>
+      <c r="D57" s="6">
+        <f t="shared" si="0"/>
+        <v>6.073857785382053E-3</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="1"/>
+        <v>6.2272504904677343E-3</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="2"/>
+        <v>2.352932197350279E-8</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
@@ -6483,6 +6563,18 @@
       <c r="C58" s="6">
         <v>0.91758199729013801</v>
       </c>
+      <c r="D58" s="6">
+        <f t="shared" si="0"/>
+        <v>6.0819972901380304E-3</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="1"/>
+        <v>6.2274249066993454E-3</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="2"/>
+        <v>2.1149191658704884E-8</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
@@ -6494,6 +6586,18 @@
       <c r="C59" s="6">
         <v>0.91758926268057095</v>
       </c>
+      <c r="D59" s="6">
+        <f t="shared" si="0"/>
+        <v>6.0892626805709726E-3</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="1"/>
+        <v>6.2275465872766471E-3</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="2"/>
+        <v>1.9122438853783666E-8</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
@@ -6505,6 +6609,18 @@
       <c r="C60" s="6">
         <v>0.91759789094005295</v>
       </c>
+      <c r="D60" s="6">
+        <f t="shared" si="0"/>
+        <v>6.0978909400529746E-3</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="1"/>
+        <v>6.2276650590143354E-3</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="2"/>
+        <v>1.6841321952197416E-8</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
@@ -6516,6 +6632,18 @@
       <c r="C61" s="6">
         <v>0.91760340511254201</v>
       </c>
+      <c r="D61" s="6">
+        <f t="shared" si="0"/>
+        <v>6.1034051125420374E-3</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="1"/>
+        <v>6.2277335398085954E-3</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="2"/>
+        <v>1.5457557826575804E-8</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
@@ -6527,6 +6655,18 @@
       <c r="C62" s="6">
         <v>0.91760623924443296</v>
       </c>
+      <c r="D62" s="6">
+        <f t="shared" si="0"/>
+        <v>6.1062392444329872E-3</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="1"/>
+        <v>6.2277731240948896E-3</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="2"/>
+        <v>1.4770483905673775E-8</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
@@ -6538,6 +6678,18 @@
       <c r="C63" s="6">
         <v>0.917607120605888</v>
       </c>
+      <c r="D63" s="6">
+        <f t="shared" si="0"/>
+        <v>6.1071206058880279E-3</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="1"/>
+        <v>6.2277960051922579E-3</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="2"/>
+        <v>1.4562551997235374E-8</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
@@ -6549,8 +6701,20 @@
       <c r="C64" s="6">
         <v>0.91760678490815295</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="6">
+        <f t="shared" si="0"/>
+        <v>6.1067849081529735E-3</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="1"/>
+        <v>6.2278092312641632E-3</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="2"/>
+        <v>1.4646886784521638E-8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>3.4019729821770199</v>
       </c>
@@ -6560,8 +6724,20 @@
       <c r="C65" s="6">
         <v>0.91760584091749398</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="6">
+        <f t="shared" si="0"/>
+        <v>6.1058409174939987E-3</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="1"/>
+        <v>6.2278168763947794E-3</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="2"/>
+        <v>1.487813454976494E-8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>3.5637144277037498</v>
       </c>
@@ -6571,8 +6747,20 @@
       <c r="C66" s="6">
         <v>0.91760442649636498</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="6">
+        <f t="shared" si="0"/>
+        <v>6.1044264963650008E-3</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="1"/>
+        <v>6.2278220746878957E-3</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="2"/>
+        <v>1.5226468749641685E-8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>3.7254558732304801</v>
       </c>
@@ -6582,8 +6770,20 @@
       <c r="C67" s="6">
         <v>0.91760324627703704</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="6">
+        <f t="shared" ref="D67:D82" si="3">C67-0.9115</f>
+        <v>6.1032462770370666E-3</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G82" si="4">$L$5*(1-EXP(-(IF(A67&lt;$L$6,0,A67-$L$6))/$L$7))</f>
+        <v>6.2278246927465987E-3</v>
+      </c>
+      <c r="H67">
+        <f t="shared" ref="H67:H82" si="5">(D67-G67)^2</f>
+        <v>1.5519781660696991E-8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>3.88719731875721</v>
       </c>
@@ -6593,8 +6793,20 @@
       <c r="C68" s="6">
         <v>0.91760250723644099</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1025072364410127E-3</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="4"/>
+        <v>6.227826011300828E-3</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="5"/>
+        <v>1.5704795332365083E-8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>4.0489387642839398</v>
       </c>
@@ -6604,8 +6816,20 @@
       <c r="C69" s="6">
         <v>0.91760218205739197</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1021820573919916E-3</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="4"/>
+        <v>6.2278266753750342E-3</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="5"/>
+        <v>1.5786570028104718E-8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>4.2106802098106701</v>
       </c>
@@ -6615,8 +6839,20 @@
       <c r="C70" s="6">
         <v>0.91760213565821303</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1021356582130482E-3</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="4"/>
+        <v>6.2278270098281357E-3</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="5"/>
+        <v>1.5798315870827577E-8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>4.4391090420971802</v>
       </c>
@@ -6626,8 +6862,20 @@
       <c r="C71" s="6">
         <v>0.91760228621797801</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1022862179780368E-3</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="4"/>
+        <v>6.2278272203724573E-3</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="5"/>
+        <v>1.576054328219588E-8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>4.6675378743836902</v>
       </c>
@@ -6637,8 +6885,20 @@
       <c r="C72" s="6">
         <v>0.917602461013587</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1024610135870239E-3</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="4"/>
+        <v>6.2278273002901799E-3</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="5"/>
+        <v>1.5716705841737916E-8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>4.8959667066702002</v>
       </c>
@@ -6648,8 +6908,20 @@
       <c r="C73" s="6">
         <v>0.91760254838714495</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1025483871449682E-3</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="4"/>
+        <v>6.2278273306250855E-3</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="5"/>
+        <v>1.5694813679494429E-8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>5.1243955389567102</v>
       </c>
@@ -6659,8 +6931,20 @@
       <c r="C74" s="6">
         <v>0.917602554827054</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1025548270540186E-3</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="4"/>
+        <v>6.2278273421395094E-3</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="5"/>
+        <v>1.5693203035844524E-8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>5.3528243712432202</v>
       </c>
@@ -6670,8 +6954,20 @@
       <c r="C75" s="6">
         <v>0.91760253131999003</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1025313199900566E-3</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="4"/>
+        <v>6.2278273465101166E-3</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="5"/>
+        <v>1.5699094261715586E-8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>5.75527595847554</v>
       </c>
@@ -6681,8 +6977,20 @@
       <c r="C76" s="6">
         <v>0.91760249807393202</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1024980739320389E-3</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="4"/>
+        <v>6.2278273486988311E-3</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="5"/>
+        <v>1.5707427113570095E-8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>6.1577275457078597</v>
       </c>
@@ -6692,8 +7000,20 @@
       <c r="C77" s="6">
         <v>0.91760251297373596</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1025129737359851E-3</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="4"/>
+        <v>6.2278273490960125E-3</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="5"/>
+        <v>1.5703692671873847E-8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>6.5601791329401804</v>
       </c>
@@ -6703,8 +7023,20 @@
       <c r="C78" s="6">
         <v>0.91760253856320295</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1025385632029749E-3</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="4"/>
+        <v>6.2278273491680886E-3</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="5"/>
+        <v>1.5697279888612049E-8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>6.9626307201725099</v>
       </c>
@@ -6714,8 +7046,20 @@
       <c r="C79" s="6">
         <v>0.91760253918300605</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1025391830060727E-3</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="4"/>
+        <v>6.2278273491811675E-3</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="5"/>
+        <v>1.5697124583518176E-8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>7.3650823074048297</v>
       </c>
@@ -6725,8 +7069,20 @@
       <c r="C80" s="6">
         <v>0.91760252255531005</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1025225553100748E-3</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="4"/>
+        <v>6.2278273491835406E-3</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="5"/>
+        <v>1.570129136767175E-8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>8.6315563163839304</v>
       </c>
@@ -6736,8 +7092,20 @@
       <c r="C81" s="6">
         <v>0.91760251298916296</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1025129891629781E-3</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="4"/>
+        <v>6.2278273491840645E-3</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="5"/>
+        <v>1.5703688827494448E-8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>10</v>
       </c>
@@ -6746,6 +7114,18 @@
       </c>
       <c r="C82" s="6">
         <v>0.91760252158595101</v>
+      </c>
+      <c r="D82" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1025215859510373E-3</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="4"/>
+        <v>6.2278273491840671E-3</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="5"/>
+        <v>1.5701534299412112E-8</v>
       </c>
     </row>
   </sheetData>
@@ -6758,8 +7138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6877,7 +7257,7 @@
       </c>
       <c r="L4">
         <f>SUM(H2:H1048576)</f>
-        <v>2.3665674649185324E-8</v>
+        <v>2.287048577419414E-8</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -6942,7 +7322,7 @@
         <v>8</v>
       </c>
       <c r="L6">
-        <v>0.18345490273341014</v>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -6971,7 +7351,7 @@
         <v>9</v>
       </c>
       <c r="L7">
-        <v>0.2251183179597776</v>
+        <v>0.18429999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -7082,11 +7462,11 @@
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>1.5106815446127851E-5</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>1.2438551035196756E-9</v>
+        <v>2.5376552823333423E-9</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -7105,11 +7485,11 @@
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>8.1345132080654209E-5</v>
+        <v>5.5469438651942637E-5</v>
       </c>
       <c r="H13">
         <f t="shared" si="2"/>
-        <v>1.0889931803180716E-12</v>
+        <v>7.2464557849612468E-10</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -7128,11 +7508,11 @@
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>1.3395310547987209E-4</v>
+        <v>1.2452526767073275E-4</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>2.96490702272637E-10</v>
+        <v>6.0700733797450563E-11</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -7151,11 +7531,11 @@
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>1.7573555113656352E-4</v>
+        <v>1.7664258920160292E-4</v>
       </c>
       <c r="H15">
         <f t="shared" si="2"/>
-        <v>5.7119759809881636E-10</v>
+        <v>6.1537626498726763E-10</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -7174,11 +7554,11 @@
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>2.0892011713013453E-4</v>
+        <v>2.1597620147078615E-4</v>
       </c>
       <c r="H16">
         <f t="shared" si="2"/>
-        <v>5.0717649070570467E-10</v>
+        <v>8.7477903040245705E-10</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -7197,11 +7577,11 @@
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>2.3527605208975569E-4</v>
+        <v>2.4566178408895744E-4</v>
       </c>
       <c r="H17">
         <f t="shared" si="2"/>
-        <v>2.5197490300594268E-10</v>
+        <v>6.8955868094753597E-10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -7220,11 +7600,11 @@
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>2.6784498142919577E-4</v>
+        <v>2.7999230424755739E-4</v>
       </c>
       <c r="H18">
         <f t="shared" si="2"/>
-        <v>1.6071538806593701E-12</v>
+        <v>1.1836541521718619E-10</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -7243,11 +7623,11 @@
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>2.8998632532677555E-4</v>
+        <v>3.0141930310782279E-4</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
-        <v>4.004922737737527E-10</v>
+        <v>7.3604822245707966E-11</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -7266,11 +7646,11 @@
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>3.0503868103922495E-4</v>
+        <v>3.1479271772655797E-4</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
-        <v>1.3071648516245572E-9</v>
+        <v>6.9699686314820076E-10</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -7289,11 +7669,11 @@
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>3.1527172802779912E-4</v>
+        <v>3.2313958047345729E-4</v>
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
-        <v>2.269111419242049E-9</v>
+        <v>1.5814412137217408E-9</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -7312,11 +7692,11 @@
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>3.2222846308447575E-4</v>
+        <v>3.2834917874748158E-4</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
-        <v>2.9003370010384969E-9</v>
+        <v>2.2785406075747221E-9</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -7335,11 +7715,11 @@
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>3.269578621288496E-4</v>
+        <v>3.3160068952460558E-4</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
-        <v>3.0414951869266805E-9</v>
+        <v>2.5509494707700233E-9</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -7358,11 +7738,11 @@
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>3.3033506863360955E-4</v>
+        <v>3.3372751217563255E-4</v>
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
-        <v>2.7168488463669589E-9</v>
+        <v>2.3747061348921611E-9</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -7381,11 +7761,11 @@
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>3.3257650863903097E-4</v>
+        <v>3.3501656589124927E-4</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
-        <v>2.1032939319140558E-9</v>
+        <v>1.8854375488002453E-9</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -7404,11 +7784,11 @@
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>3.3406414443826963E-4</v>
+        <v>3.3579785317015912E-4</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>1.4208122066703235E-9</v>
+        <v>1.2931182883668415E-9</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -7427,11 +7807,11 @@
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>3.3505148305354552E-4</v>
+        <v>3.3627138643319661E-4</v>
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>8.2947163441903101E-10</v>
+        <v>7.606920240565784E-10</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -7450,11 +7830,11 @@
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>3.3570677619835544E-4</v>
+        <v>3.365583919396932E-4</v>
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>4.0528118354439179E-10</v>
+        <v>3.717176637101455E-10</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -7473,11 +7853,11 @@
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>3.3614169193951169E-4</v>
+        <v>3.3673234415633588E-4</v>
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
-        <v>1.5287802187991967E-10</v>
+        <v>1.3862078884089361E-10</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -7496,11 +7876,11 @@
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>3.3643034397776904E-4</v>
+        <v>3.3683777549124033E-4</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>3.4880982519327251E-11</v>
+        <v>3.0234391812597305E-11</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -7519,11 +7899,11 @@
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>3.3670398018959891E-4</v>
+        <v>3.3692707771559085E-4</v>
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>1.6628776954943809E-12</v>
+        <v>2.2880303898171204E-12</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -7542,11 +7922,11 @@
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>3.3684617431444555E-4</v>
+        <v>3.3696722036883264E-4</v>
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>2.4082425068733513E-11</v>
+        <v>2.5285116338320259E-11</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -7565,11 +7945,11 @@
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>3.3692006500678375E-4</v>
+        <v>3.3698526507736044E-4</v>
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>3.3914935181119798E-11</v>
+        <v>3.4678591413814554E-11</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -7588,11 +7968,11 @@
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>3.3695846205321659E-4</v>
+        <v>3.369933764372123E-4</v>
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>2.5983847872716247E-11</v>
+        <v>2.6341014522300192E-11</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -7611,11 +7991,11 @@
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>3.3697841494752722E-4</v>
+        <v>3.3699702261185381E-4</v>
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
-        <v>1.3257859343783621E-11</v>
+        <v>1.3393711600404863E-11</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -7634,11 +8014,11 @@
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>3.3698878340105061E-4</v>
+        <v>3.3699866162057232E-4</v>
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
-        <v>4.3710907669318828E-12</v>
+        <v>4.4124934369578973E-12</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -7657,11 +8037,11 @@
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
-        <v>3.369948171020925E-4</v>
+        <v>3.3699947876709941E-4</v>
       </c>
       <c r="H37">
         <f t="shared" si="2"/>
-        <v>3.9303429742996847E-13</v>
+        <v>3.9890105232534687E-13</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -7680,11 +8060,11 @@
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
-        <v>3.3699760511801837E-4</v>
+        <v>3.3699979700544481E-4</v>
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
-        <v>5.9739671367344751E-14</v>
+        <v>5.8673006626358947E-14</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -7703,11 +8083,11 @@
       </c>
       <c r="G39">
         <f t="shared" si="1"/>
-        <v>3.3699889338748159E-4</v>
+        <v>3.3699992094361384E-4</v>
       </c>
       <c r="H39">
         <f t="shared" si="2"/>
-        <v>3.3497242744208947E-13</v>
+        <v>3.3378405004600893E-13</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -7726,11 +8106,11 @@
       </c>
       <c r="G40">
         <f t="shared" si="1"/>
-        <v>3.369994886632096E-4</v>
+        <v>3.3699996921142942E-4</v>
       </c>
       <c r="H40">
         <f t="shared" si="2"/>
-        <v>3.1214774921665572E-13</v>
+        <v>3.1161101379125877E-13</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -7749,11 +8129,11 @@
       </c>
       <c r="G41">
         <f t="shared" si="1"/>
-        <v>3.36999763724602E-4</v>
+        <v>3.3699998800936745E-4</v>
       </c>
       <c r="H41">
         <f t="shared" si="2"/>
-        <v>1.4024865948318735E-13</v>
+        <v>1.4008072145006603E-13</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -7772,11 +8152,11 @@
       </c>
       <c r="G42">
         <f t="shared" si="1"/>
-        <v>3.3699989082329934E-4</v>
+        <v>3.369999953302389E-4</v>
       </c>
       <c r="H42">
         <f t="shared" si="2"/>
-        <v>2.6279456514267638E-14</v>
+        <v>2.6245584322111602E-14</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -7795,11 +8175,11 @@
       </c>
       <c r="G43">
         <f t="shared" si="1"/>
-        <v>3.3699996694174118E-4</v>
+        <v>3.3699999891474692E-4</v>
       </c>
       <c r="H43">
         <f t="shared" si="2"/>
-        <v>8.8565422201961145E-15</v>
+        <v>8.8625611506875325E-15</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -7818,11 +8198,11 @@
       </c>
       <c r="G44">
         <f t="shared" si="1"/>
-        <v>3.3699998999009434E-4</v>
+        <v>3.3699999974778704E-4</v>
       </c>
       <c r="H44">
         <f t="shared" si="2"/>
-        <v>3.1930092518677331E-14</v>
+        <v>3.1933579816819576E-14</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -7841,11 +8221,11 @@
       </c>
       <c r="G45">
         <f t="shared" si="1"/>
-        <v>3.3699999696904144E-4</v>
+        <v>3.3699999994138565E-4</v>
       </c>
       <c r="H45">
         <f t="shared" si="2"/>
-        <v>2.0191269807315267E-14</v>
+        <v>2.0192114532525434E-14</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -7864,11 +8244,11 @@
       </c>
       <c r="G46">
         <f t="shared" si="1"/>
-        <v>3.3699999908223815E-4</v>
+        <v>3.3699999998637804E-4</v>
       </c>
       <c r="H46">
         <f t="shared" si="2"/>
-        <v>6.4965418742030202E-15</v>
+        <v>6.4966876244095604E-15</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -7887,11 +8267,11 @@
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
-        <v>3.3699999972210549E-4</v>
+        <v>3.3699999999683424E-4</v>
       </c>
       <c r="H47">
         <f t="shared" si="2"/>
-        <v>2.8677093913959205E-15</v>
+        <v>2.8677388154692462E-15</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -7910,11 +8290,11 @@
       </c>
       <c r="G48">
         <f t="shared" si="1"/>
-        <v>3.369999999694506E-4</v>
+        <v>3.3699999999978658E-4</v>
       </c>
       <c r="H48">
         <f t="shared" si="2"/>
-        <v>4.3681299139326162E-15</v>
+        <v>4.3681339238539416E-15</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -7933,11 +8313,11 @@
       </c>
       <c r="G49">
         <f t="shared" si="1"/>
-        <v>3.3699999999664164E-4</v>
+        <v>3.3699999999998559E-4</v>
       </c>
       <c r="H49">
         <f t="shared" si="2"/>
-        <v>1.1512493541389055E-14</v>
+        <v>1.1512494258976034E-14</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -7956,11 +8336,11 @@
       </c>
       <c r="G50">
         <f t="shared" si="1"/>
-        <v>3.3699999999963078E-4</v>
+        <v>3.3699999999999903E-4</v>
       </c>
       <c r="H50">
         <f t="shared" si="2"/>
-        <v>1.0977291772608631E-14</v>
+        <v>1.0977291849773478E-14</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -7979,11 +8359,11 @@
       </c>
       <c r="G51">
         <f t="shared" si="1"/>
-        <v>3.369999999999594E-4</v>
+        <v>3.3699999999999995E-4</v>
       </c>
       <c r="H51">
         <f t="shared" si="2"/>
-        <v>5.5714501007804195E-15</v>
+        <v>5.5714501068337729E-15</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -8002,11 +8382,11 @@
       </c>
       <c r="G52">
         <f t="shared" si="1"/>
-        <v>3.3699999999999556E-4</v>
+        <v>3.3700000000000001E-4</v>
       </c>
       <c r="H52">
         <f t="shared" si="2"/>
-        <v>4.1245577635264115E-15</v>
+        <v>4.1245577640973811E-15</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -8025,11 +8405,11 @@
       </c>
       <c r="G53">
         <f t="shared" si="1"/>
-        <v>3.3699999999999995E-4</v>
+        <v>3.3700000000000001E-4</v>
       </c>
       <c r="H53">
         <f t="shared" si="2"/>
-        <v>6.5371337034692137E-15</v>
+        <v>6.5371337034779796E-15</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -8087,10 +8467,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N82"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8165,17 +8545,13 @@
       <c r="C3">
         <v>0.91148404455199195</v>
       </c>
-      <c r="D3" s="6">
-        <f t="shared" ref="D3:D55" si="0">C3-0.9115</f>
-        <v>-1.5955448008031503E-5</v>
-      </c>
       <c r="G3">
-        <f t="shared" ref="G3:G55" si="1">$L$5*(1-EXP(-(IF(A3&lt;$L$6,0,A3-$L$6))/$L$7))</f>
+        <f t="shared" ref="G3:G55" si="0">$L$5*(1-EXP(-(IF(A3&lt;$L$6,0,A3-$L$6))/$L$7))</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H55" si="2">(D3-G3)^2</f>
-        <v>2.5457632113699647E-10</v>
+        <f t="shared" ref="H3:H55" si="1">(D3-G3)^2</f>
+        <v>0</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>6</v>
@@ -8183,7 +8559,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>1.0014437198306899E-3</v>
+        <v>4.91842337505706E-3</v>
       </c>
       <c r="B4">
         <v>441.14891098236001</v>
@@ -8191,29 +8567,25 @@
       <c r="C4">
         <v>0.91148413860946798</v>
       </c>
-      <c r="D4" s="6">
-        <f t="shared" si="0"/>
-        <v>-1.5861390532001529E-5</v>
-      </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="2"/>
-        <v>2.5158370960866774E-10</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L4">
         <f>SUM(H2:H1048576)</f>
-        <v>6.7687887277872318E-7</v>
+        <v>4.4550790552419718E-6</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>2.0028874396613799E-3</v>
+        <v>9.8368467501141303E-3</v>
       </c>
       <c r="B5">
         <v>441.14943407981298</v>
@@ -8221,35 +8593,31 @@
       <c r="C5">
         <v>0.91148433961687803</v>
       </c>
-      <c r="D5" s="6">
-        <f t="shared" si="0"/>
-        <v>-1.5660383121951504E-5</v>
-      </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
-        <v>2.4524759952630356E-10</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L5">
-        <v>3.3700000000000001E-4</v>
+        <v>3.4000000000000002E-4</v>
       </c>
       <c r="M5" t="s">
         <v>13</v>
       </c>
       <c r="N5">
         <f>L5/0.1</f>
-        <v>3.3699999999999997E-3</v>
+        <v>3.4000000000000002E-3</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>3.00433115949208E-3</v>
+        <v>1.4755270125171201E-2</v>
       </c>
       <c r="B6">
         <v>441.14997362953898</v>
@@ -8257,28 +8625,24 @@
       <c r="C6">
         <v>0.911484647763249</v>
       </c>
-      <c r="D6" s="6">
-        <f t="shared" si="0"/>
-        <v>-1.5352236750976189E-5</v>
-      </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H6">
-        <f t="shared" si="2"/>
-        <v>2.3569117325802396E-10</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L6">
-        <v>0.18345490273341014</v>
+        <v>0.2122</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>7.5862184192504603E-3</v>
+        <v>4.9487280823212097E-2</v>
       </c>
       <c r="B7">
         <v>441.15417526618802</v>
@@ -8286,28 +8650,24 @@
       <c r="C7">
         <v>0.91148948682133002</v>
       </c>
-      <c r="D7" s="6">
-        <f t="shared" si="0"/>
-        <v>-1.051317866995749E-5</v>
-      </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
-        <v>1.1052692574644915E-10</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="L7">
-        <v>0.2251183179597776</v>
+        <v>0.18429999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>1.2168105679008801E-2</v>
+        <v>8.4219291521253001E-2</v>
       </c>
       <c r="B8">
         <v>441.15900938759199</v>
@@ -8315,22 +8675,18 @@
       <c r="C8">
         <v>0.91149879651614996</v>
       </c>
-      <c r="D8" s="6">
-        <f t="shared" si="0"/>
-        <v>-1.2034838500207812E-6</v>
-      </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
-        <v>1.4483733772608421E-12</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>1.6749992938767201E-2</v>
+        <v>0.111609353954937</v>
       </c>
       <c r="B9">
         <v>441.16318597516499</v>
@@ -8338,22 +8694,18 @@
       <c r="C9">
         <v>0.91150892001269301</v>
       </c>
-      <c r="D9" s="6">
-        <f t="shared" si="0"/>
-        <v>8.9200126930366608E-6</v>
-      </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="2"/>
-        <v>7.9566626443935137E-11</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>2.13318801985256E-2</v>
+        <v>0.13899941638862101</v>
       </c>
       <c r="B10">
         <v>441.16760109876202</v>
@@ -8361,22 +8713,18 @@
       <c r="C10">
         <v>0.91152110565573496</v>
       </c>
-      <c r="D10" s="6">
-        <f t="shared" si="0"/>
-        <v>2.1105655734987572E-5</v>
-      </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
-        <v>4.4544870400381379E-10</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>3.32468704828284E-2</v>
+        <v>0.16638947882230501</v>
       </c>
       <c r="B11">
         <v>441.17218839012997</v>
@@ -8384,22 +8732,18 @@
       <c r="C11">
         <v>0.91153502686602605</v>
       </c>
-      <c r="D11" s="6">
-        <f t="shared" si="0"/>
-        <v>3.5026866026077741E-5</v>
-      </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
-        <v>1.2268813436087992E-9</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>4.51618607671311E-2</v>
+        <v>0.19377954125598901</v>
       </c>
       <c r="B12">
         <v>441.17688702362301</v>
@@ -8407,22 +8751,18 @@
       <c r="C12">
         <v>0.91155037514548198</v>
       </c>
-      <c r="D12" s="6">
-        <f t="shared" si="0"/>
-        <v>5.0375145482006722E-5</v>
-      </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
-        <v>2.5376552823333423E-9</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>5.7076851051433897E-2</v>
+        <v>0.24564486633477201</v>
       </c>
       <c r="B13">
         <v>441.18590767901998</v>
@@ -8430,22 +8770,18 @@
       <c r="C13">
         <v>0.91158238868044095</v>
       </c>
-      <c r="D13" s="6">
-        <f t="shared" si="0"/>
-        <v>8.2388680440970141E-5</v>
-      </c>
       <c r="G13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.6425205371993719E-5</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
-        <v>6.7878946648042959E-9</v>
+        <f t="shared" si="1"/>
+        <v>3.1838038012716691E-9</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>6.8991841335736701E-2</v>
+        <v>0.297510191413555</v>
       </c>
       <c r="B14">
         <v>441.194808203874</v>
@@ -8453,22 +8789,18 @@
       <c r="C14">
         <v>0.91161673420010603</v>
       </c>
-      <c r="D14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.1673420010605007E-4</v>
-      </c>
       <c r="G14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.2598245854586926E-4</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
-        <v>1.362687347439934E-8</v>
+        <f t="shared" si="1"/>
+        <v>1.5871579861261668E-8</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>9.30170939382024E-2</v>
+        <v>0.349375516492338</v>
       </c>
       <c r="B15">
         <v>441.20331554161999</v>
@@ -8476,22 +8808,18 @@
       <c r="C15">
         <v>0.91165183581059195</v>
       </c>
-      <c r="D15" s="6">
-        <f t="shared" si="0"/>
-        <v>1.5183581059197149E-4</v>
-      </c>
       <c r="G15">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.7847821132990446E-4</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
-        <v>2.3054113378121042E-8</v>
+        <f t="shared" si="1"/>
+        <v>3.1854471919522037E-8</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>0.117042346540668</v>
+        <v>0.401240841571121</v>
       </c>
       <c r="B16">
         <v>441.21122392458699</v>
@@ -8499,22 +8827,18 @@
       <c r="C16">
         <v>0.91168639953785902</v>
       </c>
-      <c r="D16" s="6">
-        <f t="shared" si="0"/>
-        <v>1.8639953785903884E-4</v>
-      </c>
       <c r="G16">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.1809743052870933E-4</v>
       </c>
       <c r="H16">
-        <f t="shared" si="2"/>
-        <v>3.4744787714063253E-8</v>
+        <f t="shared" si="1"/>
+        <v>4.7566489203225191E-8</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>0.14106759914313399</v>
+        <v>0.453106166649904</v>
       </c>
       <c r="B17">
         <v>441.21838815710697</v>
@@ -8522,22 +8846,18 @@
       <c r="C17">
         <v>0.91171940233472404</v>
       </c>
-      <c r="D17" s="6">
-        <f t="shared" si="0"/>
-        <v>2.1940233472406145E-4</v>
-      </c>
       <c r="G17">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.4799856436672748E-4</v>
       </c>
       <c r="H17">
-        <f t="shared" si="2"/>
-        <v>4.8137384482369103E-8</v>
+        <f t="shared" si="1"/>
+        <v>6.150328792795788E-8</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>0.16509285174560001</v>
+        <v>0.539982054148746</v>
       </c>
       <c r="B18">
         <v>441.22847557783001</v>
@@ -8545,22 +8865,18 @@
       <c r="C18">
         <v>0.91176911271715899</v>
       </c>
-      <c r="D18" s="6">
-        <f t="shared" si="0"/>
-        <v>2.6911271715901464E-4</v>
-      </c>
       <c r="G18">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.8257836329453152E-4</v>
       </c>
       <c r="H18">
-        <f t="shared" si="2"/>
-        <v>7.2421654536707816E-8</v>
+        <f t="shared" si="1"/>
+        <v>7.985053140221624E-8</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>0.189118104348065</v>
+        <v>0.62685794164758901</v>
       </c>
       <c r="B19">
         <v>441.23605133605002</v>
@@ -8568,22 +8884,18 @@
       <c r="C19">
         <v>0.91180999862838696</v>
       </c>
-      <c r="D19" s="6">
-        <f t="shared" si="0"/>
-        <v>3.0999862838698711E-4</v>
-      </c>
       <c r="G19">
-        <f t="shared" si="1"/>
-        <v>8.3720124189070084E-6</v>
+        <f t="shared" si="0"/>
+        <v>3.0416094662829007E-4</v>
       </c>
       <c r="H19">
-        <f t="shared" si="2"/>
-        <v>9.097861546035566E-8</v>
+        <f t="shared" si="1"/>
+        <v>9.2513881453817524E-8</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>0.22731265406023399</v>
+        <v>0.71373382914643102</v>
       </c>
       <c r="B20">
         <v>441.241213149901</v>
@@ -8591,22 +8903,18 @@
       <c r="C20">
         <v>0.91184119341588299</v>
       </c>
-      <c r="D20" s="6">
-        <f t="shared" si="0"/>
-        <v>3.4119341588301211E-4</v>
-      </c>
       <c r="G20">
-        <f t="shared" si="1"/>
-        <v>5.965504975787341E-5</v>
+        <f t="shared" si="0"/>
+        <v>3.1763146750468792E-4</v>
       </c>
       <c r="H20">
-        <f t="shared" si="2"/>
-        <v>7.9263851600412637E-8</v>
+        <f t="shared" si="1"/>
+        <v>1.0088974914918161E-7</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>0.265507203772402</v>
+        <v>0.80060971664527403</v>
       </c>
       <c r="B21">
         <v>441.24423342473602</v>
@@ -8614,22 +8922,18 @@
       <c r="C21">
         <v>0.91186290691900296</v>
       </c>
-      <c r="D21" s="6">
-        <f t="shared" si="0"/>
-        <v>3.62906919002981E-4</v>
-      </c>
       <c r="G21">
-        <f t="shared" si="1"/>
-        <v>1.029352692660512E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.2603893800418313E-4</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
-        <v>6.7585258666940907E-8</v>
+        <f t="shared" si="1"/>
+        <v>1.0630138909489556E-7</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>0.30370175348457001</v>
+        <v>0.88748560414411604</v>
       </c>
       <c r="B22">
         <v>441.24548350702202</v>
@@ -8637,22 +8941,18 @@
       <c r="C22">
         <v>0.91187608324004099</v>
       </c>
-      <c r="D22" s="6">
-        <f t="shared" si="0"/>
-        <v>3.7608324004101412E-4</v>
-      </c>
       <c r="G22">
-        <f t="shared" si="1"/>
-        <v>1.3946152624835377E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3128636390912584E-4</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
-        <v>5.5989835438175667E-8</v>
+        <f t="shared" si="1"/>
+        <v>1.0975065491212976E-7</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>0.33491955499458298</v>
+        <v>0.97436149164295904</v>
       </c>
       <c r="B23">
         <v>441.24537492669799</v>
@@ -8660,22 +8960,18 @@
       <c r="C23">
         <v>0.91188210761450295</v>
       </c>
-      <c r="D23" s="6">
-        <f t="shared" si="0"/>
-        <v>3.8210761450296893E-4</v>
-      </c>
       <c r="G23">
-        <f t="shared" si="1"/>
-        <v>1.6504023812375317E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3456148436652354E-4</v>
       </c>
       <c r="H23">
-        <f t="shared" si="2"/>
-        <v>4.7118245888156113E-8</v>
+        <f t="shared" si="1"/>
+        <v>1.1193138682153157E-7</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>0.366137356504595</v>
+        <v>1.06664432724486</v>
       </c>
       <c r="B24">
         <v>441.244227767155</v>
@@ -8683,22 +8979,18 @@
       <c r="C24">
         <v>0.91188245846881399</v>
       </c>
-      <c r="D24" s="6">
-        <f t="shared" si="0"/>
-        <v>3.8245846881401757E-4</v>
-      </c>
       <c r="G24">
-        <f t="shared" si="1"/>
-        <v>1.8730683318069722E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3670375017804782E-4</v>
       </c>
       <c r="H24">
-        <f t="shared" si="2"/>
-        <v>3.8084160890360228E-8</v>
+        <f t="shared" si="1"/>
+        <v>1.1336941538396124E-7</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>0.39735515801460802</v>
+        <v>1.1589271628467701</v>
       </c>
       <c r="B25">
         <v>441.24244614443103</v>
@@ -8706,22 +8998,18 @@
       <c r="C25">
         <v>0.91187843819125003</v>
       </c>
-      <c r="D25" s="6">
-        <f t="shared" si="0"/>
-        <v>3.7843819125005229E-4</v>
-      </c>
       <c r="G25">
-        <f t="shared" si="1"/>
-        <v>2.0669018828650299E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3800216389526602E-4</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
-        <v>2.9497376521967338E-8</v>
+        <f t="shared" si="1"/>
+        <v>1.1424546279788227E-7</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>0.42857295952461999</v>
+        <v>1.25120999844867</v>
       </c>
       <c r="B26">
         <v>441.24039014264599</v>
@@ -8729,22 +9017,18 @@
       <c r="C26">
         <v>0.91187175780712404</v>
       </c>
-      <c r="D26" s="6">
-        <f t="shared" si="0"/>
-        <v>3.7175780712406237E-4</v>
-      </c>
       <c r="G26">
-        <f t="shared" si="1"/>
-        <v>2.2356364622638553E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3878912421176412E-4</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
-        <v>2.1961509324166531E-8</v>
+        <f t="shared" si="1"/>
+        <v>1.1477807068417413E-7</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>0.45979076103463301</v>
+        <v>1.3434928340505701</v>
       </c>
       <c r="B27">
         <v>441.23833510911197</v>
@@ -8752,22 +9036,18 @@
       <c r="C27">
         <v>0.91186385203225695</v>
       </c>
-      <c r="D27" s="6">
-        <f t="shared" si="0"/>
-        <v>3.6385203225697271E-4</v>
-      </c>
       <c r="G27">
-        <f t="shared" si="1"/>
-        <v>2.382522066585124E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3926609586689235E-4</v>
       </c>
       <c r="H27">
-        <f t="shared" si="2"/>
-        <v>1.5775316190363646E-8</v>
+        <f t="shared" si="1"/>
+        <v>1.1510148380476339E-7</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>0.49936874012619498</v>
+        <v>1.4357756696524699</v>
       </c>
       <c r="B28">
         <v>441.236473654338</v>
@@ -8775,22 +9055,18 @@
       <c r="C28">
         <v>0.91185583837284501</v>
       </c>
-      <c r="D28" s="6">
-        <f t="shared" si="0"/>
-        <v>3.5583837284502984E-4</v>
-      </c>
       <c r="G28">
-        <f t="shared" si="1"/>
-        <v>2.5417256234187114E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3955518536102109E-4</v>
       </c>
       <c r="H28">
-        <f t="shared" si="2"/>
-        <v>1.0335937025264174E-8</v>
+        <f t="shared" si="1"/>
+        <v>1.1529772390555738E-7</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>0.53894671921775805</v>
+        <v>1.52805850525438</v>
       </c>
       <c r="B29">
         <v>441.234922041966</v>
@@ -8798,22 +9074,18 @@
       <c r="C29">
         <v>0.91184850607715995</v>
       </c>
-      <c r="D29" s="6">
-        <f t="shared" si="0"/>
-        <v>3.4850607715997128E-4</v>
-      </c>
       <c r="G29">
-        <f t="shared" si="1"/>
-        <v>2.6752620016240014E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3973040066934612E-4</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
-        <v>6.5577404785417528E-9</v>
+        <f t="shared" si="1"/>
+        <v>1.1541674513895445E-7</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>0.57852469830931996</v>
+        <v>1.6203413408562799</v>
       </c>
       <c r="B30">
         <v>441.23373125910098</v>
@@ -8821,22 +9093,18 @@
       <c r="C30">
         <v>0.91184233635638201</v>
       </c>
-      <c r="D30" s="6">
-        <f t="shared" si="0"/>
-        <v>3.4233635638203364E-4</v>
-      </c>
       <c r="G30">
-        <f t="shared" si="1"/>
-        <v>2.7872693251967061E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3983659755610593E-4</v>
       </c>
       <c r="H30">
-        <f t="shared" si="2"/>
-        <v>4.0461588041017583E-9</v>
+        <f t="shared" si="1"/>
+        <v>1.1548891303851071E-7</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>0.61810267740088298</v>
+        <v>1.7677052167426099</v>
       </c>
       <c r="B31">
         <v>441.232578292185</v>
@@ -8844,22 +9112,18 @@
       <c r="C31">
         <v>0.91183541445403804</v>
       </c>
-      <c r="D31" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3541445403806325E-4</v>
-      </c>
       <c r="G31">
-        <f t="shared" si="1"/>
-        <v>2.8812185598736765E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3992654821655559E-4</v>
       </c>
       <c r="H31">
-        <f t="shared" si="2"/>
-        <v>2.2365898303846575E-9</v>
+        <f t="shared" si="1"/>
+        <v>1.1555005818242229E-7</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>0.657680656492445</v>
+        <v>1.91506909262894</v>
       </c>
       <c r="B32">
         <v>441.23218562387899</v>
@@ -8867,22 +9131,18 @@
       <c r="C32">
         <v>0.91183193878956603</v>
       </c>
-      <c r="D32" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3193878956605527E-4</v>
-      </c>
       <c r="G32">
-        <f t="shared" si="1"/>
-        <v>2.9600210739848053E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3996698235128807E-4</v>
       </c>
       <c r="H32">
-        <f t="shared" si="2"/>
-        <v>1.291445125213284E-9</v>
+        <f t="shared" si="1"/>
+        <v>1.1557754908904101E-7</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>0.69725863558400802</v>
+        <v>2.06243296851527</v>
       </c>
       <c r="B33">
         <v>441.23229115114998</v>
@@ -8890,22 +9150,18 @@
       <c r="C33">
         <v>0.91183109641192805</v>
       </c>
-      <c r="D33" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3109641192807793E-4</v>
-      </c>
       <c r="G33">
-        <f t="shared" si="1"/>
-        <v>3.0261188580868952E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3998515808500023E-4</v>
       </c>
       <c r="H33">
-        <f t="shared" si="2"/>
-        <v>8.113682282461203E-10</v>
+        <f t="shared" si="1"/>
+        <v>1.155899077180826E-7</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>0.77075750511395402</v>
+        <v>2.2097968444016001</v>
       </c>
       <c r="B34">
         <v>441.232643305002</v>
@@ -8913,22 +9169,18 @@
       <c r="C34">
         <v>0.91183186102663205</v>
       </c>
-      <c r="D34" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3186102663207429E-4</v>
-      </c>
       <c r="G34">
-        <f t="shared" si="1"/>
-        <v>3.1219063924263268E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999332834258481E-4</v>
       </c>
       <c r="H34">
-        <f t="shared" si="2"/>
-        <v>3.8692414005070326E-10</v>
+        <f t="shared" si="1"/>
+        <v>1.1559546331746869E-7</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>0.84425637464390002</v>
+        <v>2.3571607202879301</v>
       </c>
       <c r="B35">
         <v>441.23305560243102</v>
@@ -8936,22 +9188,18 @@
       <c r="C35">
         <v>0.91183333728059901</v>
       </c>
-      <c r="D35" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3333728059903311E-4</v>
-      </c>
       <c r="G35">
-        <f t="shared" si="1"/>
-        <v>3.1910124644332112E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999700099261677E-4</v>
       </c>
       <c r="H35">
-        <f t="shared" si="2"/>
-        <v>2.0266466848259853E-10</v>
+        <f t="shared" si="1"/>
+        <v>1.1559796068397345E-7</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>0.91775524417384602</v>
+        <v>2.5045245961742602</v>
       </c>
       <c r="B36">
         <v>441.23341592894798</v>
@@ -8959,22 +9207,18 @@
       <c r="C36">
         <v>0.91183489806802898</v>
       </c>
-      <c r="D36" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3489806802899924E-4</v>
-      </c>
       <c r="G36">
-        <f t="shared" si="1"/>
-        <v>3.2408691521656439E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999865190240971E-4</v>
       </c>
       <c r="H36">
-        <f t="shared" si="2"/>
-        <v>1.1688102513381805E-10</v>
+        <f t="shared" si="1"/>
+        <v>1.1559908329545597E-7</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>0.99125411370379202</v>
+        <v>2.67832277870686</v>
       </c>
       <c r="B37">
         <v>441.23370566181501</v>
@@ -8982,22 +9226,18 @@
       <c r="C37">
         <v>0.91183636789262701</v>
       </c>
-      <c r="D37" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3636789262703193E-4</v>
-      </c>
       <c r="G37">
-        <f t="shared" si="1"/>
-        <v>3.2768383403927167E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999947498235353E-4</v>
       </c>
       <c r="H37">
-        <f t="shared" si="2"/>
-        <v>7.5412873555652617E-11</v>
+        <f t="shared" si="1"/>
+        <v>1.1559964298827605E-7</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>1.0481872795190601</v>
+        <v>2.8521209612394598</v>
       </c>
       <c r="B38">
         <v>441.23384398433598</v>
@@ -9005,22 +9245,18 @@
       <c r="C38">
         <v>0.91183724202212102</v>
       </c>
-      <c r="D38" s="6">
-        <f t="shared" si="0"/>
-        <v>3.372420221210426E-4</v>
-      </c>
       <c r="G38">
-        <f t="shared" si="1"/>
-        <v>3.2976559682684189E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999979553147263E-4</v>
       </c>
       <c r="H38">
-        <f t="shared" si="2"/>
-        <v>5.5896935179764064E-11</v>
+        <f t="shared" si="1"/>
+        <v>1.1559986096144319E-7</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>1.10512044533432</v>
+        <v>3.0259191437720601</v>
       </c>
       <c r="B39">
         <v>441.23386921552299</v>
@@ -9028,22 +9264,18 @@
       <c r="C39">
         <v>0.91183757766141305</v>
       </c>
-      <c r="D39" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3757766141306877E-4</v>
-      </c>
       <c r="G39">
-        <f t="shared" si="1"/>
-        <v>3.3138217508227915E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999992036957429E-4</v>
       </c>
       <c r="H39">
-        <f t="shared" si="2"/>
-        <v>3.8384050875001054E-11</v>
+        <f t="shared" si="1"/>
+        <v>1.1559994585131686E-7</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>1.16205361114959</v>
+        <v>3.1997173263046599</v>
       </c>
       <c r="B40">
         <v>441.23383259747601</v>
@@ -9051,22 +9283,18 @@
       <c r="C40">
         <v>0.91183755819050605</v>
       </c>
-      <c r="D40" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3755819050607094E-4</v>
-      </c>
       <c r="G40">
-        <f t="shared" si="1"/>
-        <v>3.3263751756008555E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999996898786928E-4</v>
       </c>
       <c r="H40">
-        <f t="shared" si="2"/>
-        <v>2.4213022241352584E-11</v>
+        <f t="shared" si="1"/>
+        <v>1.1559997891175208E-7</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>1.2189867769648599</v>
+        <v>3.3735155088372601</v>
       </c>
       <c r="B41">
         <v>441.233776508186</v>
@@ -9074,22 +9302,18 @@
       <c r="C41">
         <v>0.91183737426160105</v>
       </c>
-      <c r="D41" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3737426160107553E-4</v>
-      </c>
       <c r="G41">
-        <f t="shared" si="1"/>
-        <v>3.3361234493468639E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999998792230181E-4</v>
       </c>
       <c r="H41">
-        <f t="shared" si="2"/>
-        <v>1.4152017004856355E-11</v>
+        <f t="shared" si="1"/>
+        <v>1.1559999178716537E-7</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>1.27591994278012</v>
+        <v>3.54731369136986</v>
       </c>
       <c r="B42">
         <v>441.23372640437498</v>
@@ -9097,22 +9321,18 @@
       <c r="C42">
         <v>0.91183716200022003</v>
       </c>
-      <c r="D42" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3716200022004816E-4</v>
-      </c>
       <c r="G42">
-        <f t="shared" si="1"/>
-        <v>3.3436934027824525E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999529633115E-4</v>
       </c>
       <c r="H42">
-        <f t="shared" si="2"/>
-        <v>7.7989495505506658E-12</v>
+        <f t="shared" si="1"/>
+        <v>1.1559999680150521E-7</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>1.3328531085953901</v>
+        <v>3.81626170252092</v>
       </c>
       <c r="B43">
         <v>441.23367736982698</v>
@@ -9120,22 +9340,18 @@
       <c r="C43">
         <v>0.91183690585773802</v>
       </c>
-      <c r="D43" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3690585773804571E-4</v>
-      </c>
       <c r="G43">
-        <f t="shared" si="1"/>
-        <v>3.3495717968971497E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999890686674E-4</v>
       </c>
       <c r="H43">
-        <f t="shared" si="2"/>
-        <v>3.7973461360461073E-12</v>
+        <f t="shared" si="1"/>
+        <v>1.1559999925666938E-7</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>1.3897862744106499</v>
+        <v>4.0852097136719898</v>
       </c>
       <c r="B44">
         <v>441.23366887696801</v>
@@ -9143,22 +9359,18 @@
       <c r="C44">
         <v>0.91183682130005606</v>
       </c>
-      <c r="D44" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3682130005607824E-4</v>
-      </c>
       <c r="G44">
-        <f t="shared" si="1"/>
-        <v>3.3541366225148668E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999974595568E-4</v>
       </c>
       <c r="H44">
-        <f t="shared" si="2"/>
-        <v>1.9814441889153647E-12</v>
+        <f t="shared" si="1"/>
+        <v>1.1559999982724986E-7</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>1.4860985568396501</v>
+        <v>4.3541577248230601</v>
       </c>
       <c r="B45">
         <v>441.23368196766597</v>
@@ -9166,22 +9378,18 @@
       <c r="C45">
         <v>0.91183685790098101</v>
       </c>
-      <c r="D45" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3685790098103574E-4</v>
-      </c>
       <c r="G45">
-        <f t="shared" si="1"/>
-        <v>3.359658307518656E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999994096007E-4</v>
       </c>
       <c r="H45">
-        <f t="shared" si="2"/>
-        <v>7.9578929377166591E-13</v>
+        <f t="shared" si="1"/>
+        <v>1.1559999995985285E-7</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>1.58241083926864</v>
+        <v>4.6231057359741303</v>
       </c>
       <c r="B46">
         <v>441.23369498334699</v>
@@ -9189,22 +9397,18 @@
       <c r="C46">
         <v>0.91183691939795397</v>
       </c>
-      <c r="D46" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3691939795399417E-4</v>
-      </c>
       <c r="G46">
-        <f t="shared" si="1"/>
-        <v>3.3632580181314523E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999998627912E-4</v>
       </c>
       <c r="H46">
-        <f t="shared" si="2"/>
-        <v>3.5235637843075179E-13</v>
+        <f t="shared" si="1"/>
+        <v>1.155999999906698E-7</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>1.65736610205237</v>
+        <v>4.8920537471251899</v>
       </c>
       <c r="B47">
         <v>441.23369833270402</v>
@@ -9212,22 +9416,18 @@
       <c r="C47">
         <v>0.91183694644872404</v>
       </c>
-      <c r="D47" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3694644872406254E-4</v>
-      </c>
       <c r="G47">
-        <f t="shared" si="1"/>
-        <v>3.3651673522036753E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999999681128E-4</v>
       </c>
       <c r="H47">
-        <f t="shared" si="2"/>
-        <v>1.8465369525784634E-13</v>
+        <f t="shared" si="1"/>
+        <v>1.1559999999783166E-7</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>1.7323213648361</v>
+        <v>5.3890916164626397</v>
       </c>
       <c r="B48">
         <v>441.23369255673202</v>
@@ -9235,22 +9435,18 @@
       <c r="C48">
         <v>0.91183693390814002</v>
       </c>
-      <c r="D48" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3693390814004687E-4</v>
-      </c>
       <c r="G48">
-        <f t="shared" si="1"/>
-        <v>3.3665359615052843E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999999978503E-4</v>
       </c>
       <c r="H48">
-        <f t="shared" si="2"/>
-        <v>7.8574811467785503E-14</v>
+        <f t="shared" si="1"/>
+        <v>1.1559999999985382E-7</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>1.80727662761984</v>
+        <v>5.8861294858000903</v>
       </c>
       <c r="B49">
         <v>441.23368537477802</v>
@@ -9258,22 +9454,18 @@
       <c r="C49">
         <v>0.91183689270370805</v>
       </c>
-      <c r="D49" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3689270370806934E-4</v>
-      </c>
       <c r="G49">
-        <f t="shared" si="1"/>
-        <v>3.3675169796768559E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999999998555E-4</v>
       </c>
       <c r="H49">
-        <f t="shared" si="2"/>
-        <v>1.9882618821169996E-14</v>
+        <f t="shared" si="1"/>
+        <v>1.1559999999999017E-7</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>1.88223189040357</v>
+        <v>6.3831673551375303</v>
       </c>
       <c r="B50">
         <v>441.23368844641402</v>
@@ -9281,22 +9473,18 @@
       <c r="C50">
         <v>0.91183689522742795</v>
       </c>
-      <c r="D50" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3689522742796907E-4</v>
-      </c>
       <c r="G50">
-        <f t="shared" si="1"/>
-        <v>3.36822017280277E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999999999905E-4</v>
       </c>
       <c r="H50">
-        <f t="shared" si="2"/>
-        <v>5.359725725093962E-15</v>
+        <f t="shared" si="1"/>
+        <v>1.1559999999999935E-7</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>1.9571871531873</v>
+        <v>6.8802052244749801</v>
       </c>
       <c r="B51">
         <v>441.23369477670099</v>
@@ -9304,22 +9492,18 @@
       <c r="C51">
         <v>0.91183692535785299</v>
       </c>
-      <c r="D51" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3692535785301292E-4</v>
-      </c>
       <c r="G51">
-        <f t="shared" si="1"/>
-        <v>3.3687242211340466E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.3999999999999997E-4</v>
       </c>
       <c r="H51">
-        <f t="shared" si="2"/>
-        <v>2.8021925278729204E-15</v>
+        <f t="shared" si="1"/>
+        <v>1.1559999999999998E-7</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>2.03214241597103</v>
+        <v>7.37724309381242</v>
       </c>
       <c r="B52">
         <v>441.233695306485</v>
@@ -9327,22 +9511,18 @@
       <c r="C52">
         <v>0.91183693577727998</v>
       </c>
-      <c r="D52" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3693577728000079E-4</v>
-      </c>
       <c r="G52">
-        <f t="shared" si="1"/>
-        <v>3.3690855226185183E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.4000000000000002E-4</v>
       </c>
       <c r="H52">
-        <f t="shared" si="2"/>
-        <v>7.4120161321131095E-16</v>
+        <f t="shared" si="1"/>
+        <v>1.1560000000000002E-7</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>2.1170446810321399</v>
+        <v>8.3353221296594207</v>
       </c>
       <c r="B53">
         <v>441.233690691128</v>
@@ -9350,22 +9530,18 @@
       <c r="C53">
         <v>0.91183691914745701</v>
       </c>
-      <c r="D53" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3691914745703766E-4</v>
-      </c>
       <c r="G53">
-        <f t="shared" si="1"/>
-        <v>3.3693728362576262E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.4000000000000002E-4</v>
       </c>
       <c r="H53">
-        <f t="shared" si="2"/>
-        <v>3.2892061602031084E-16</v>
+        <f t="shared" si="1"/>
+        <v>1.1560000000000002E-7</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>2.2019469460932402</v>
+        <v>9.2934011655064204</v>
       </c>
       <c r="B54">
         <v>441.23368899971098</v>
@@ -9373,22 +9549,18 @@
       <c r="C54">
         <v>0.91183690392305305</v>
       </c>
-      <c r="D54" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3690392305307792E-4</v>
-      </c>
       <c r="G54">
-        <f t="shared" si="1"/>
-        <v>3.3695698807125103E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.4000000000000002E-4</v>
       </c>
       <c r="H54">
-        <f t="shared" si="2"/>
-        <v>2.8158961537118814E-15</v>
+        <f t="shared" si="1"/>
+        <v>1.1560000000000002E-7</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>2.2868492111543399</v>
+        <v>10</v>
       </c>
       <c r="B55">
         <v>441.233692295026</v>
@@ -9396,233 +9568,13 @@
       <c r="C55">
         <v>0.91183691666590005</v>
       </c>
-      <c r="D55" s="6">
-        <f t="shared" si="0"/>
-        <v>3.3691666590007774E-4</v>
-      </c>
       <c r="G55">
-        <f t="shared" si="1"/>
-        <v>3.3697050170649684E-4</v>
+        <f t="shared" si="0"/>
+        <v>3.4000000000000002E-4</v>
       </c>
       <c r="H55">
-        <f t="shared" si="2"/>
-        <v>2.8982940527953484E-15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
-        <v>2.3717514762154499</v>
-      </c>
-      <c r="B56">
-        <v>442.67032232060598</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
-        <v>2.4566537412765501</v>
-      </c>
-      <c r="B57">
-        <v>442.67253899489401</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>2.5415560063376499</v>
-      </c>
-      <c r="B58">
-        <v>442.67449450515301</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>2.6264582713987501</v>
-      </c>
-      <c r="B59">
-        <v>442.67610293438401</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>2.7557107231951301</v>
-      </c>
-      <c r="B60">
-        <v>442.67782768843801</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>2.8849631749915101</v>
-      </c>
-      <c r="B61">
-        <v>442.67876600949899</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>3.0142156267878901</v>
-      </c>
-      <c r="B62">
-        <v>442.67911159464097</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
-        <v>3.1434680785842599</v>
-      </c>
-      <c r="B63">
-        <v>442.67907631972201</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
-        <v>3.2727205303806399</v>
-      </c>
-      <c r="B64">
-        <v>442.67884004948098</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
-        <v>3.4019729821770199</v>
-      </c>
-      <c r="B65">
-        <v>442.67853480274999</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
-        <v>3.5637144277037498</v>
-      </c>
-      <c r="B66">
-        <v>442.67817398641603</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
-        <v>3.7254558732304801</v>
-      </c>
-      <c r="B67">
-        <v>442.67791839974899</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
-        <v>3.88719731875721</v>
-      </c>
-      <c r="B68">
-        <v>442.677784476917</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
-        <v>4.0489387642839398</v>
-      </c>
-      <c r="B69">
-        <v>442.67774475439103</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
-        <v>4.2106802098106701</v>
-      </c>
-      <c r="B70">
-        <v>442.67775850328098</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
-        <v>4.4391090420971802</v>
-      </c>
-      <c r="B71">
-        <v>442.67780931189401</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
-        <v>4.6675378743836902</v>
-      </c>
-      <c r="B72">
-        <v>442.67784964442302</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
-        <v>4.8959667066702002</v>
-      </c>
-      <c r="B73">
-        <v>442.67786432231998</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
-        <v>5.1243955389567102</v>
-      </c>
-      <c r="B74">
-        <v>442.67786187534398</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
-        <v>5.3528243712432202</v>
-      </c>
-      <c r="B75">
-        <v>442.67785563413901</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
-        <v>5.75527595847554</v>
-      </c>
-      <c r="B76">
-        <v>442.67784924433499</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
-        <v>6.1577275457078597</v>
-      </c>
-      <c r="B77">
-        <v>442.67785388178902</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
-        <v>6.5601791329401804</v>
-      </c>
-      <c r="B78">
-        <v>442.67785890467002</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
-        <v>6.9626307201725099</v>
-      </c>
-      <c r="B79">
-        <v>442.67785776157899</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
-        <v>7.3650823074048297</v>
-      </c>
-      <c r="B80">
-        <v>442.67785390399303</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
-        <v>8.6315563163839304</v>
-      </c>
-      <c r="B81">
-        <v>442.67785272217901</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
-        <v>10</v>
-      </c>
-      <c r="B82">
-        <v>442.67785490413303</v>
+        <f t="shared" si="1"/>
+        <v>1.1560000000000002E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>